<commit_message>
update data collection model
</commit_message>
<xml_diff>
--- a/curation/draft/collections_specialization_draft.xlsx
+++ b/curation/draft/collections_specialization_draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3411B454-6B96-44B7-82EC-A487900E7F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84069719-1C71-47CA-9BCB-1BB1DF4D9BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA29263D-F7AA-4D0C-AE9B-6B008D3B18BE}"/>
+    <workbookView xWindow="28680" yWindow="915" windowWidth="29040" windowHeight="15840" xr2:uid="{FA29263D-F7AA-4D0C-AE9B-6B008D3B18BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_VS" sheetId="16" r:id="rId1"/>
@@ -826,10 +826,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CAAE8E-5C13-4AF4-981F-FF7495593B56}">
   <dimension ref="A1:AG12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="AH1" sqref="AH1:AL1048576"/>
+      <selection pane="bottomLeft" activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>